<commit_message>
modified:   app.py 	modified:   cpf_test_site/cpf.html
</commit_message>
<xml_diff>
--- a/planilha_fechamento.xlsx
+++ b/planilha_fechamento.xlsx
@@ -1,66 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>CPF</t>
-  </si>
-  <si>
-    <t>Vencimento</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Data Pagamento</t>
-  </si>
-  <si>
-    <t>Método Pagamento</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -83,27 +57,89 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,46 +427,638 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="11.14785714285714" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="16.71928571428571" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="18.86214285714286" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CPF</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Vencimento</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Data Pagamento</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Método Pagamento</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Noah da Mota</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>747.91</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>472.963.815-82</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Santos</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>123.2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>231.659.708-40</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Dr. Felipe Farias</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>285.56</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>487.039.126-04</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>07/02/2024</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Luigi Barros</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>349.87</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>179.432.680-40</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>29/06/2024</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Stella da Luz</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>449.42</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>821.074.653-71</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>16/07/2024</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Elisa da Cunha</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>655.34</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>281.597.640-49</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>07/05/2024</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Rodrigo Fernandes</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>615.39</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>358.170.962-77</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>13/07/2024</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Dra. Alícia Monteiro</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>726.4299999999999</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>098.132.475-41</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>26/06/2024</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Eduardo Farias</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>370.38</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>203.546.178-26</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>23/06/2024</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Dr. Gustavo Costa</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>949.45</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>916.253.408-42</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sarah Fogaça</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>661.26</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>197.382.460-40</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>27/06/2024</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Thomas Costa</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>375.81</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>732.481.056-07</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>07/06/2024</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>João Felipe Aragão</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>666.9299999999999</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>839.140.256-89</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>07/08/2024</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Noah da Mota</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>747.91</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>472.963.815-82</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>07/04/2024</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Carlos Eduardo Santos</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>123.2</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>231.659.708-40</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Dr. Felipe Farias</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>285.56</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>487.039.126-04</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>07/02/2024</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Luigi Barros</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>349.87</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>179.432.680-40</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>29/06/2024</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Stella da Luz</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>449.42</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>821.074.653-71</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>16/07/2024</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Elisa da Cunha</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>655.34</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>281.597.640-49</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>07/05/2024</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Rodrigo Fernandes</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>615.39</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>358.170.962-77</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>13/07/2024</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Dra. Alícia Monteiro</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>726.4299999999999</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>098.132.475-41</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>26/06/2024</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Eduardo Farias</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>370.38</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>203.546.178-26</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>23/06/2024</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Dr. Gustavo Costa</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>949.45</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>916.253.408-42</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>pendente</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>